<commit_message>
Added Student details in excel file.
</commit_message>
<xml_diff>
--- a/1.xlsx
+++ b/1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Excel Testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Test\Test3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E636B090-451F-4471-9CC1-E6FEEBF27567}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E939EA2-30A7-4DF0-BCE5-FBDA39770DED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>roll number</t>
   </si>
@@ -52,6 +52,18 @@
   </si>
   <si>
     <t>ece</t>
+  </si>
+  <si>
+    <t>Manoj</t>
+  </si>
+  <si>
+    <t>Final</t>
+  </si>
+  <si>
+    <t>JNTU</t>
+  </si>
+  <si>
+    <t>CSE</t>
   </si>
 </sst>
 </file>
@@ -396,19 +408,19 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.21875" customWidth="1"/>
+    <col min="1" max="1" width="16.28515625" customWidth="1"/>
     <col min="2" max="2" width="25" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" customWidth="1"/>
-    <col min="4" max="4" width="26.6640625" customWidth="1"/>
-    <col min="5" max="5" width="17.21875" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" customWidth="1"/>
+    <col min="4" max="4" width="26.7109375" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -425,7 +437,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="3" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -442,7 +454,24 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D13" s="2"/>
     </row>
   </sheetData>

</xml_diff>